<commit_message>
- Do not convert `NAs` for readIndividualCharacteristicsFromXLS as it is now solved in ospsuite-r - Add test for individual characteristics with empty numerical cells
</commit_message>
<xml_diff>
--- a/tests/data/IndividualPhysiology.xlsx
+++ b/tests/data/IndividualPhysiology.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\OSPS\Repos\esqlabsR\tests\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5444D520-EDA0-4F7B-B38D-23BD2723C264}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7F92B68-44C9-4BA8-9C09-AD53CF745D9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Individuals" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="13">
   <si>
     <t>Human</t>
   </si>
@@ -70,6 +70,9 @@
   </si>
   <si>
     <t>Woerle_2003_H</t>
+  </si>
+  <si>
+    <t>Individual_with_NAs</t>
   </si>
 </sst>
 </file>
@@ -394,31 +397,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M6" sqref="M6"/>
+      <selection activeCell="B4" sqref="B4:D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="35.453125" customWidth="1"/>
-    <col min="2" max="2" width="6.90625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="35.42578125" customWidth="1"/>
+    <col min="2" max="2" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.26953125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.36328125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.36328125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="4.1796875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.7265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="4.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="11" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11" customWidth="1"/>
-    <col min="12" max="12" width="8.453125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.7265625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.453125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -441,7 +444,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -464,7 +467,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>11</v>
       </c>
@@ -485,6 +488,20 @@
       </c>
       <c r="G3" s="1">
         <v>43</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -495,15 +512,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010011DB5BA7A27696418C6D2C8B46A68E83" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="b6960b7ce0e258e5d224c1a71edff679">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="398d2b5b-77f8-4c5f-a794-3d35ce849315" xmlns:ns3="1c52e43a-7a2d-43c4-9ede-f251c929c0a1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e7db7ba54f101f424e932c64edcbdaa0" ns2:_="" ns3:_="">
     <xsd:import namespace="398d2b5b-77f8-4c5f-a794-3d35ce849315"/>
@@ -720,6 +728,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -727,14 +744,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{78CA0B51-7456-4883-901E-100C95177B36}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0EEA776C-4DAB-4C30-9CC1-14DE8CBA854F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -753,6 +762,14 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{78CA0B51-7456-4883-901E-100C95177B36}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{028903B1-0B22-4BE6-8A73-043144867A27}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Revert changes from 183 (#188)
* Replace NAs in units of readParametersFromXLS to allow the unit "" for the dimension "Dimensionless"

* Export readExcel

* Fixes #182
Convert NA to NULL in createIndividualCharacteristics

* Fix applying derived parameters also to human species

* Fix #184
readOSPSTimeValues - dataType not set

* - Do not convert `NAs` for readIndividualCharacteristicsFromXLS as it is now solved in ospsuite-r
- Add test for individual characteristics with empty numerical cells
</commit_message>
<xml_diff>
--- a/tests/data/IndividualPhysiology.xlsx
+++ b/tests/data/IndividualPhysiology.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\OSPS\Repos\esqlabsR\tests\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5444D520-EDA0-4F7B-B38D-23BD2723C264}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7F92B68-44C9-4BA8-9C09-AD53CF745D9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Individuals" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="13">
   <si>
     <t>Human</t>
   </si>
@@ -70,6 +70,9 @@
   </si>
   <si>
     <t>Woerle_2003_H</t>
+  </si>
+  <si>
+    <t>Individual_with_NAs</t>
   </si>
 </sst>
 </file>
@@ -394,31 +397,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M6" sqref="M6"/>
+      <selection activeCell="B4" sqref="B4:D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="35.453125" customWidth="1"/>
-    <col min="2" max="2" width="6.90625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="35.42578125" customWidth="1"/>
+    <col min="2" max="2" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.26953125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.36328125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.36328125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="4.1796875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.7265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="4.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="11" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11" customWidth="1"/>
-    <col min="12" max="12" width="8.453125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.7265625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.453125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -441,7 +444,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -464,7 +467,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>11</v>
       </c>
@@ -485,6 +488,20 @@
       </c>
       <c r="G3" s="1">
         <v>43</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -495,15 +512,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010011DB5BA7A27696418C6D2C8B46A68E83" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="b6960b7ce0e258e5d224c1a71edff679">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="398d2b5b-77f8-4c5f-a794-3d35ce849315" xmlns:ns3="1c52e43a-7a2d-43c4-9ede-f251c929c0a1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e7db7ba54f101f424e932c64edcbdaa0" ns2:_="" ns3:_="">
     <xsd:import namespace="398d2b5b-77f8-4c5f-a794-3d35ce849315"/>
@@ -720,6 +728,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -727,14 +744,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{78CA0B51-7456-4883-901E-100C95177B36}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0EEA776C-4DAB-4C30-9CC1-14DE8CBA854F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -753,6 +762,14 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{78CA0B51-7456-4883-901E-100C95177B36}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{028903B1-0B22-4BE6-8A73-043144867A27}">
   <ds:schemaRefs>

</xml_diff>